<commit_message>
fix cer + csv name page 0 to 25
</commit_message>
<xml_diff>
--- a/data/transcriptions/transcription_ex12.xlsx
+++ b/data/transcriptions/transcription_ex12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/seorin_kim_vub_be/Documents/img-analysis_seorin_project/data/transcriptions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Documents\GitHub\img-analysis_seorin_project\data\transcriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="718" documentId="13_ncr:1_{10B1438D-2B05-4A31-AE33-93986825B1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A418ED6-00A7-0E4A-BE1C-165C688EC014}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FC3A0-C6BF-4AB3-9F50-9AEC82B7FA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
   </bookViews>
   <sheets>
     <sheet name="IMG_2024_03_19_11_47_29_885" sheetId="2" r:id="rId1"/>
@@ -365,7 +365,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -634,10 +634,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -959,18 +955,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB076F5B-4564-1543-8968-7E29FE54F40E}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.875" customWidth="1"/>
+    <col min="7" max="7" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="27" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +1014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="28"/>
       <c r="B2" s="30"/>
       <c r="C2" s="4" t="s">
@@ -1070,7 +1066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20">
       <c r="A3" s="19" t="s">
         <v>29</v>
       </c>
@@ -1118,7 +1114,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1166,7 +1162,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20">
       <c r="A5" s="2"/>
       <c r="B5" s="11"/>
       <c r="C5" s="16" t="s">
@@ -1187,7 +1183,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20">
       <c r="A6" s="2"/>
       <c r="B6" s="11"/>
       <c r="C6" s="16" t="s">
@@ -1207,7 +1203,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20">
       <c r="A7" s="2"/>
       <c r="B7" s="11"/>
       <c r="C7" s="16" t="s">
@@ -1228,7 +1224,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20">
       <c r="A8" s="2">
         <v>442</v>
       </c>
@@ -1278,7 +1274,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -1330,7 +1326,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20">
       <c r="A10" s="2"/>
       <c r="B10" s="11"/>
       <c r="C10" s="16"/>
@@ -1354,7 +1350,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
         <v>50</v>
       </c>
@@ -1406,7 +1402,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1458,7 +1454,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20">
       <c r="A13" s="2"/>
       <c r="B13" s="11"/>
       <c r="C13" s="16" t="s">
@@ -1479,7 +1475,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20">
       <c r="A14" s="2"/>
       <c r="B14" s="11"/>
       <c r="C14" s="18" t="s">
@@ -1499,7 +1495,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1545,7 +1541,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20">
       <c r="A16" s="2">
         <v>443</v>
       </c>
@@ -1592,7 +1588,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20">
       <c r="A17" s="2"/>
       <c r="B17" s="11"/>
       <c r="C17" s="18"/>
@@ -1611,7 +1607,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20">
       <c r="A18" s="2"/>
       <c r="B18" s="11"/>
       <c r="C18" s="18"/>
@@ -1630,7 +1626,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20">
       <c r="A19" s="2"/>
       <c r="B19" s="11"/>
       <c r="C19" s="3"/>
@@ -1649,7 +1645,7 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
@@ -1667,7 +1663,7 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
@@ -1686,7 +1682,7 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
@@ -1704,7 +1700,7 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20">
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
       <c r="E23" s="1"/>
@@ -1722,7 +1718,7 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="E24" s="1"/>
@@ -1740,7 +1736,7 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20">
       <c r="A25" s="6"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>

</xml_diff>